<commit_message>
test cases without any pair info
</commit_message>
<xml_diff>
--- a/tests/data_files/FileFastq_pairing.xlsx
+++ b/tests/data_files/FileFastq_pairing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>#Field Name:</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>test_lab:f3_2</t>
+  </si>
+  <si>
+    <t>test_lab:f5_1, test_lab:alt_f5_1</t>
   </si>
 </sst>
 </file>
@@ -187,8 +190,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,7 +216,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -217,6 +224,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -224,6 +233,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,10 +567,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -784,6 +795,22 @@
       <c r="F12" s="2" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="B14" s="2"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
added single sided connection
</commit_message>
<xml_diff>
--- a/tests/data_files/FileFastq_pairing.xlsx
+++ b/tests/data_files/FileFastq_pairing.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
   <si>
     <t>#Field Name:</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>test_lab:f5_1, test_lab:alt_f5_1</t>
+  </si>
+  <si>
+    <t>test_lab:f6_1, test_lab:alt_f6_1</t>
+  </si>
+  <si>
+    <t>test_lab:f6_2, test_lab:alt_f6_2</t>
+  </si>
+  <si>
+    <t>test_lab:f6_1</t>
   </si>
 </sst>
 </file>
@@ -190,8 +199,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -216,7 +227,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -226,6 +237,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -235,6 +247,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,10 +580,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -807,10 +820,36 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="2"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="B15" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
adding another type of pairing that does not work when one sided
</commit_message>
<xml_diff>
--- a/tests/data_files/FileFastq_pairing.xlsx
+++ b/tests/data_files/FileFastq_pairing.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10512"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrew/Documents/work/Submit4DN/tests/data_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FD5790-E4FA-4548-8CD6-980E6D9BAE1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="3140" windowWidth="43760" windowHeight="23880" tabRatio="500"/>
+    <workbookView xWindow="-34880" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FileFastq" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
   <si>
     <t>#Field Name:</t>
   </si>
@@ -154,12 +160,21 @@
   </si>
   <si>
     <t>test_lab:f6_1</t>
+  </si>
+  <si>
+    <t>test_lab:f7_1, test_lab:alt_f7_1</t>
+  </si>
+  <si>
+    <t>test_lab:f7_2, test_lab:alt_f7_2</t>
+  </si>
+  <si>
+    <t>test_lab:alt_f7_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -252,6 +267,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -576,24 +599,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
     <col min="2" max="2" width="80" customWidth="1"/>
     <col min="6" max="6" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -633,7 +656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -651,7 +674,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -671,7 +694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>27</v>
@@ -689,7 +712,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
       <c r="B6" s="2" t="s">
         <v>28</v>
@@ -707,7 +730,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
@@ -724,7 +747,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
@@ -741,7 +764,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B9" s="2" t="s">
         <v>31</v>
       </c>
@@ -758,7 +781,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
@@ -775,7 +798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
         <v>33</v>
       </c>
@@ -792,7 +815,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
         <v>34</v>
       </c>
@@ -809,7 +832,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
@@ -819,7 +842,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
@@ -829,12 +852,10 @@
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
@@ -849,6 +870,34 @@
       </c>
       <c r="F15" s="2" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>